<commit_message>
add reference design (BQ76952EVM)
</commit_message>
<xml_diff>
--- a/00_PROJECT_RESEARCH/Power_Distribution.xlsx
+++ b/00_PROJECT_RESEARCH/Power_Distribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5e506f2770d8f1de/PERSONAL PROJECTS/SPRINTER VAN BATTERY/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\SprinterVanBattery\00_PROJECT_RESEARCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="277" documentId="8_{979755B1-F12E-47C7-897A-DCB3A8C54412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{046690C4-8864-4E7D-BAB1-15C9741BF7D7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F50B30-8AE9-4E25-AFA9-CF01BBDBB774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18240" yWindow="312" windowWidth="21504" windowHeight="16740" tabRatio="671" firstSheet="7" xr2:uid="{8657B37E-F4DC-4EC1-A8DB-FB2E6FC22FCF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="671" activeTab="4" xr2:uid="{8657B37E-F4DC-4EC1-A8DB-FB2E6FC22FCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Load Info" sheetId="1" r:id="rId1"/>
@@ -271,7 +271,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -857,21 +857,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2024A6-18B7-4C2A-B90B-BAF72E6597E1}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="A2:E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -885,7 +885,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>4</v>
       </c>
@@ -894,7 +894,7 @@
       <c r="D2" s="23"/>
       <c r="E2" s="25"/>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>5</v>
       </c>
@@ -913,7 +913,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>6</v>
       </c>
@@ -932,7 +932,7 @@
         <v>20.83</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>7</v>
       </c>
@@ -951,7 +951,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>8</v>
       </c>
@@ -970,7 +970,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -985,13 +984,13 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -999,7 +998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1022,12 +1021,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
@@ -1048,9 +1047,9 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
@@ -1067,19 +1066,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194B1715-89B1-4EBA-B1B3-6FC5DDCD609A}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -1122,7 +1121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="26">
         <v>2</v>
       </c>
@@ -1139,7 +1138,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="26">
         <v>3</v>
       </c>
@@ -1154,7 +1153,7 @@
       <c r="F4" s="34"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:7" ht="15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -1177,7 +1176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="26">
         <v>5</v>
       </c>
@@ -1194,7 +1193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="26">
         <v>6</v>
       </c>
@@ -1211,7 +1210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="26">
         <v>7</v>
       </c>
@@ -1228,7 +1227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="26">
         <v>8</v>
       </c>
@@ -1245,7 +1244,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>9</v>
       </c>
@@ -1262,12 +1261,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G11">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G13">
         <f>SUM(G2:G11)</f>
         <v>34</v>
@@ -1294,12 +1293,12 @@
       <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1315,12 +1314,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>37</v>
       </c>
@@ -1341,25 +1340,25 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="31.9" thickBot="1">
+    <row r="2" spans="1:9" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A2" s="9" t="s">
         <v>39</v>
       </c>
@@ -1369,7 +1368,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>41</v>
       </c>
@@ -1391,7 +1390,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>45</v>
       </c>
@@ -1415,7 +1414,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>48</v>
       </c>
@@ -1434,7 +1433,7 @@
       </c>
       <c r="I5" s="17"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>50</v>
       </c>
@@ -1453,7 +1452,7 @@
       </c>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1">
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>52</v>
       </c>
@@ -1473,17 +1472,17 @@
       <c r="H7" s="6"/>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="31.15">
+    <row r="9" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A9" s="11" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>55</v>
       </c>
@@ -1495,7 +1494,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>57</v>
       </c>
@@ -1507,7 +1506,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>59</v>
       </c>
@@ -1519,7 +1518,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>61</v>
       </c>
@@ -1531,11 +1530,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>62</v>
       </c>
@@ -1547,7 +1546,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>63</v>
       </c>
@@ -1559,24 +1558,24 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1">
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
     </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1">
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="31.15">
+    <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A20" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>65</v>
       </c>
@@ -1587,7 +1586,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>52</v>
       </c>
@@ -1596,17 +1595,17 @@
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="31.15">
+    <row r="24" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A24" s="11" t="s">
         <v>54</v>
       </c>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>41</v>
       </c>
@@ -1618,7 +1617,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>57</v>
       </c>
@@ -1630,7 +1629,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>59</v>
       </c>
@@ -1642,7 +1641,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>61</v>
       </c>
@@ -1654,11 +1653,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>62</v>
       </c>
@@ -1670,7 +1669,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>63</v>
       </c>
@@ -1682,7 +1681,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1">
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
@@ -1701,37 +1700,37 @@
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="14" max="14" width="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="14:14" ht="14.45" customHeight="1">
+    <row r="1" spans="14:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N1" s="20" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="14:14">
+    <row r="2" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N2" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="14:14">
+    <row r="3" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N3" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="14:14">
+    <row r="4" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N4" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="14:14">
+    <row r="5" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N5" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="14:14">
+    <row r="6" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N6" s="8" t="s">
         <v>72</v>
       </c>

</xml_diff>